<commit_message>
Time Record Manager - 18 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0002649_TimeRecordManager_VerifyTimeEntriesareRoundOffToFirstDecimalPlace.xlsx
+++ b/TestData/LV_TMTT0002649_TimeRecordManager_VerifyTimeEntriesareRoundOffToFirstDecimalPlace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5C13D2-5649-49AF-8AA0-609DE124B374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96551F1A-83B3-4D99-BBBC-0932F531C10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -97,12 +97,6 @@
     <t>SummaryLogTimeEntryRoundOff</t>
   </si>
   <si>
-    <t>4.455</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
     <t>DetailLogTIme</t>
   </si>
   <si>
@@ -131,6 +125,12 @@
   </si>
   <si>
     <t>120286</t>
+  </si>
+  <si>
+    <t>4.777</t>
+  </si>
+  <si>
+    <t>4.8</t>
   </si>
 </sst>
 </file>
@@ -464,20 +464,20 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -494,19 +494,19 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -522,16 +522,16 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -547,19 +547,19 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -582,9 +582,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -599,13 +599,13 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
@@ -625,15 +625,15 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -647,9 +647,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -674,45 +674,45 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Time Record Manager - 21 Jan 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0002649_TimeRecordManager_VerifyTimeEntriesareRoundOffToFirstDecimalPlace.xlsx
+++ b/TestData/LV_TMTT0002649_TimeRecordManager_VerifyTimeEntriesareRoundOffToFirstDecimalPlace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96551F1A-83B3-4D99-BBBC-0932F531C10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6858CBC-7F32-4A41-A53B-EA32C5DC53EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -127,10 +127,10 @@
     <t>120286</t>
   </si>
   <si>
+    <t>4.8</t>
+  </si>
+  <si>
     <t>4.777</t>
-  </si>
-  <si>
-    <t>4.8</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,7 +674,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,13 +706,13 @@
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>